<commit_message>
Config editor GUI, max mails, feedback loop, frame icons and sorted periods
</commit_message>
<xml_diff>
--- a/lijst.xlsx
+++ b/lijst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581C69E6-34E1-4EE6-8E8A-7816123F2F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8805E919-51EE-46EE-A5A0-BB10C4A7CFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9F5E0E70-7DD8-4E25-81DA-AF72ECB2F422}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{9F5E0E70-7DD8-4E25-81DA-AF72ECB2F422}"/>
   </bookViews>
   <sheets>
     <sheet name="Gefilterd" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Keppens</t>
   </si>
@@ -566,7 +566,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A2" sqref="A2:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -649,7 +649,9 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -657,7 +659,7 @@
         <v>49</v>
       </c>
       <c r="D2" s="1">
-        <v>24945</v>
+        <v>40285</v>
       </c>
       <c r="E2" t="s">
         <v>50</v>
@@ -728,6 +730,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B3839F4F-5790-445D-9B5E-0849697298AE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>